<commit_message>
Server: Gacha Table 수정
</commit_message>
<xml_diff>
--- a/Server/Server/GameData/Gacha.xlsx
+++ b/Server/Server/GameData/Gacha.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\porject\fix\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lcmbb\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B9A1C8-C70A-420E-A7EB-F2F9278B7F75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6FD21BF-BB9F-4FEB-9BC3-C164139EDE70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="14980" windowHeight="15370" activeTab="1" xr2:uid="{4FE2F6FA-A971-4D00-9C9F-70C15B0F2373}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{4FE2F6FA-A971-4D00-9C9F-70C15B0F2373}"/>
   </bookViews>
   <sheets>
     <sheet name="GachaGroup" sheetId="1" r:id="rId1"/>
@@ -37,6 +37,24 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={24C381FC-5ADD-4E23-8CF8-0EB0DC782001}</author>
+  </authors>
+  <commentList>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{24C381FC-5ADD-4E23-8CF8-0EB0DC782001}">
+      <text>
+        <t>[스레드 댓글]
+사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
+댓글:
+    가챠 종류</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={900EBAE7-FA83-4C9D-95AE-AEA38F8BCB92}</author>
@@ -64,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
   <si>
     <t>Index</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -78,26 +96,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>기본 상자</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Gacha_Group</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>고급상자</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pay_Item_Index</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pay_Item_Value</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Reward_Item_Index</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -114,10 +116,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>다이아 상자</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>하얀색 스킨</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -178,10 +176,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">고급상자 티켓 확률 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>나뭇가지</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -199,6 +193,38 @@
   </si>
   <si>
     <t>후라이팬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>냥냥가챠</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>울트라 냥냥가챠</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pay_Item1_Index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pay_Item1_Value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pay_Item2_Index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pay_Item2_Value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">냥냥가챠 뽑기권 확률 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">울트라 냥냥가챠 뽑기권 확률 </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -238,7 +264,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -257,6 +283,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -272,17 +304,26 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -305,6 +346,7 @@
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <person displayName="경천 강" id="{DEFDF8BA-08CC-4ECF-8F60-F1EEA043FDC6}" userId="9a4f2fb646cdd437" providerId="Windows Live"/>
+  <person displayName="창민 이" id="{C63CAAFE-5126-48D0-AB92-6D66926E1E10}" userId="fda0e400ac064334" providerId="Windows Live"/>
 </personList>
 </file>
 
@@ -625,6 +667,14 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="C1" dT="2024-11-07T06:07:01.26" personId="{C63CAAFE-5126-48D0-AB92-6D66926E1E10}" id="{24C381FC-5ADD-4E23-8CF8-0EB0DC782001}">
+    <text>가챠 종류</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="C1" dT="2024-10-04T05:16:23.08" personId="{DEFDF8BA-08CC-4ECF-8F60-F1EEA043FDC6}" id="{900EBAE7-FA83-4C9D-95AE-AEA38F8BCB92}">
     <text>상자종류</text>
   </threadedComment>
@@ -635,159 +685,158 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0A44DD5-7D06-438B-9FE5-436D9EFF504F}">
-  <dimension ref="A1:G4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0A44DD5-7D06-438B-9FE5-436D9EFF504F}">
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.08203125" customWidth="1"/>
-    <col min="2" max="5" width="24" customWidth="1"/>
-    <col min="6" max="7" width="12.83203125" customWidth="1"/>
+    <col min="1" max="1" width="7.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="16.3984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="15.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A2">
+    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="2">
         <v>100011</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2">
-        <v>1001</v>
-      </c>
-      <c r="D2">
+      <c r="B2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1001</v>
+      </c>
+      <c r="D2" s="2">
         <v>100001</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>1000</v>
       </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A3">
+      <c r="F2" s="2">
+        <v>100004</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="4">
+        <v>45292</v>
+      </c>
+      <c r="I2" s="4">
+        <v>73050</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="2">
         <v>100012</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3">
+      <c r="B3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="2">
         <v>1002</v>
       </c>
-      <c r="D3">
-        <v>100003</v>
-      </c>
-      <c r="E3">
+      <c r="D3" s="2">
+        <v>100002</v>
+      </c>
+      <c r="E3" s="2">
         <v>100</v>
       </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A4">
-        <v>100013</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4">
-        <v>1003</v>
-      </c>
-      <c r="D4">
-        <v>100002</v>
-      </c>
-      <c r="E4">
-        <v>5</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
+      <c r="F3" s="2">
+        <v>100005</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1</v>
+      </c>
+      <c r="H3" s="4">
+        <v>45292</v>
+      </c>
+      <c r="I3" s="4">
+        <v>73050</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BA63B6B-56B9-4D2F-ADF1-A0D874D69E23}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.08203125" customWidth="1"/>
-    <col min="2" max="6" width="24" customWidth="1"/>
+    <col min="1" max="1" width="10.09765625" customWidth="1"/>
+    <col min="2" max="2" width="26.796875" customWidth="1"/>
+    <col min="3" max="6" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1001001</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C2">
         <v>1001</v>
@@ -802,32 +851,32 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>1001002</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C3">
         <v>1001</v>
       </c>
       <c r="D3">
-        <v>4000</v>
+        <v>1000</v>
       </c>
       <c r="E3">
-        <v>100003</v>
+        <v>100004</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>1001003</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C4">
         <v>1001</v>
@@ -842,12 +891,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>1001004</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C5">
         <v>1001</v>
@@ -862,12 +911,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>1001005</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C6">
         <v>1001</v>
@@ -882,12 +931,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>1001006</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C7">
         <v>1001</v>
@@ -902,12 +951,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>1001007</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C8">
         <v>1001</v>
@@ -922,12 +971,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>1001008</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C9">
         <v>1001</v>
@@ -942,12 +991,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>1001009</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C10">
         <v>1001</v>
@@ -962,12 +1011,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>1001010</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C11">
         <v>1001</v>
@@ -982,12 +1031,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>1001011</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C12">
         <v>1001</v>
@@ -1002,12 +1051,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>1001012</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C13">
         <v>1001</v>
@@ -1022,12 +1071,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>1001013</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C14">
         <v>1001</v>
@@ -1042,12 +1091,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>1001014</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C15">
         <v>1001</v>
@@ -1062,12 +1111,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>1001015</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C16">
         <v>1001</v>
@@ -1082,12 +1131,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>1001016</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C17">
         <v>1001</v>
@@ -1102,263 +1151,223 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A18">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A18" s="5">
         <v>1002001</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="5">
+        <v>1002</v>
+      </c>
+      <c r="D18" s="5">
+        <v>3000</v>
+      </c>
+      <c r="E18" s="5">
+        <v>100001</v>
+      </c>
+      <c r="F18" s="5">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A19" s="5">
+        <v>1002002</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="5">
+        <v>1002</v>
+      </c>
+      <c r="D19" s="5">
+        <v>3000</v>
+      </c>
+      <c r="E19" s="5">
+        <v>100005</v>
+      </c>
+      <c r="F19" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A20" s="5">
+        <v>1002003</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="5">
+        <v>1002</v>
+      </c>
+      <c r="D20" s="5">
+        <v>3000</v>
+      </c>
+      <c r="E20" s="5">
+        <v>322001</v>
+      </c>
+      <c r="F20" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A21" s="5">
+        <v>1002004</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="5">
+        <v>1002</v>
+      </c>
+      <c r="D21" s="5">
+        <v>3000</v>
+      </c>
+      <c r="E21" s="5">
+        <v>331001</v>
+      </c>
+      <c r="F21" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A22" s="5">
+        <v>1002005</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="5">
+        <v>1002</v>
+      </c>
+      <c r="D22" s="5">
+        <v>3000</v>
+      </c>
+      <c r="E22" s="5">
+        <v>331002</v>
+      </c>
+      <c r="F22" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A23" s="5">
+        <v>1002006</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="5">
+        <v>1002</v>
+      </c>
+      <c r="D23" s="5">
+        <v>3000</v>
+      </c>
+      <c r="E23" s="5">
+        <v>331003</v>
+      </c>
+      <c r="F23" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A24" s="5">
+        <v>1002007</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C18">
+      <c r="C24" s="5">
         <v>1002</v>
       </c>
-      <c r="D18">
+      <c r="D24" s="5">
         <v>3000</v>
       </c>
-      <c r="E18">
-        <v>100001</v>
-      </c>
-      <c r="F18">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A19">
-        <v>1002002</v>
-      </c>
-      <c r="B19" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19">
+      <c r="E24" s="5">
+        <v>332001</v>
+      </c>
+      <c r="F24" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A25" s="5">
+        <v>1002008</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" s="5">
         <v>1002</v>
       </c>
-      <c r="D19">
+      <c r="D25" s="5">
         <v>3000</v>
       </c>
-      <c r="E19">
-        <v>100003</v>
-      </c>
-      <c r="F19">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A20">
-        <v>1002003</v>
-      </c>
-      <c r="B20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20">
+      <c r="E25" s="5">
+        <v>332002</v>
+      </c>
+      <c r="F25" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A26" s="5">
+        <v>1002009</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="5">
         <v>1002</v>
       </c>
-      <c r="D20">
+      <c r="D26" s="5">
         <v>3000</v>
       </c>
-      <c r="E20">
-        <v>322001</v>
-      </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A21">
-        <v>1002004</v>
-      </c>
-      <c r="B21" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21">
+      <c r="E26" s="5">
+        <v>332003</v>
+      </c>
+      <c r="F26" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A27" s="5">
+        <v>1002010</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="5">
         <v>1002</v>
       </c>
-      <c r="D21">
+      <c r="D27" s="5">
         <v>3000</v>
       </c>
-      <c r="E21">
-        <v>331001</v>
-      </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A22">
-        <v>1002005</v>
-      </c>
-      <c r="B22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22">
+      <c r="E27" s="5">
+        <v>313001</v>
+      </c>
+      <c r="F27" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A28" s="5">
+        <v>1002011</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="5">
         <v>1002</v>
       </c>
-      <c r="D22">
+      <c r="D28" s="5">
         <v>3000</v>
       </c>
-      <c r="E22">
-        <v>331002</v>
-      </c>
-      <c r="F22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A23">
-        <v>1002006</v>
-      </c>
-      <c r="B23" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23">
-        <v>1002</v>
-      </c>
-      <c r="D23">
-        <v>3000</v>
-      </c>
-      <c r="E23">
-        <v>331003</v>
-      </c>
-      <c r="F23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A24">
-        <v>1002007</v>
-      </c>
-      <c r="B24" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24">
-        <v>1002</v>
-      </c>
-      <c r="D24">
-        <v>3000</v>
-      </c>
-      <c r="E24">
-        <v>332001</v>
-      </c>
-      <c r="F24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A25">
-        <v>1002008</v>
-      </c>
-      <c r="B25" t="s">
-        <v>29</v>
-      </c>
-      <c r="C25">
-        <v>1002</v>
-      </c>
-      <c r="D25">
-        <v>3000</v>
-      </c>
-      <c r="E25">
-        <v>332002</v>
-      </c>
-      <c r="F25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A26">
-        <v>1002009</v>
-      </c>
-      <c r="B26" t="s">
-        <v>30</v>
-      </c>
-      <c r="C26">
-        <v>1002</v>
-      </c>
-      <c r="D26">
-        <v>3000</v>
-      </c>
-      <c r="E26">
-        <v>332003</v>
-      </c>
-      <c r="F26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A27">
-        <v>1002010</v>
-      </c>
-      <c r="B27" t="s">
-        <v>31</v>
-      </c>
-      <c r="C27">
-        <v>1002</v>
-      </c>
-      <c r="D27">
-        <v>3000</v>
-      </c>
-      <c r="E27">
-        <v>313001</v>
-      </c>
-      <c r="F27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A28">
-        <v>1002011</v>
-      </c>
-      <c r="B28" t="s">
-        <v>32</v>
-      </c>
-      <c r="C28">
-        <v>1002</v>
-      </c>
-      <c r="D28">
-        <v>3000</v>
-      </c>
-      <c r="E28">
+      <c r="E28" s="5">
         <v>333001</v>
       </c>
-      <c r="F28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A29">
-        <v>1003001</v>
-      </c>
-      <c r="B29" t="s">
-        <v>31</v>
-      </c>
-      <c r="C29">
-        <v>1003</v>
-      </c>
-      <c r="D29">
-        <v>5000</v>
-      </c>
-      <c r="E29">
-        <v>313001</v>
-      </c>
-      <c r="F29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A30">
-        <v>1003002</v>
-      </c>
-      <c r="B30" t="s">
-        <v>32</v>
-      </c>
-      <c r="C30">
-        <v>1003</v>
-      </c>
-      <c r="D30">
-        <v>5000</v>
-      </c>
-      <c r="E30">
-        <v>333001</v>
-      </c>
-      <c r="F30">
+      <c r="F28" s="5">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Server: Gacha table 추가된 시트 반영
</commit_message>
<xml_diff>
--- a/Server/Server/GameData/Gacha.xlsx
+++ b/Server/Server/GameData/Gacha.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lcmbb\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lcmbb\OneDrive\바탕 화면\아웃게임 기획 정리\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6FD21BF-BB9F-4FEB-9BC3-C164139EDE70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E7051A-B389-424B-B9EA-875F1F08E314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{4FE2F6FA-A971-4D00-9C9F-70C15B0F2373}"/>
+    <workbookView xWindow="3585" yWindow="990" windowWidth="15525" windowHeight="14505" activeTab="2" xr2:uid="{4FE2F6FA-A971-4D00-9C9F-70C15B0F2373}"/>
   </bookViews>
   <sheets>
     <sheet name="GachaGroup" sheetId="1" r:id="rId1"/>
     <sheet name="GachaGroup_Item" sheetId="5" r:id="rId2"/>
+    <sheet name="When_Dup" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -81,8 +82,28 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={262C3525-30B3-4A0E-9280-CCBF27DD5D25}</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{262C3525-30B3-4A0E-9280-CCBF27DD5D25}">
+      <text>
+        <t>[스레드 댓글]
+사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
+댓글:
+    Normal = 1
+Rare = 2
+Unique = 3</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
   <si>
     <t>Index</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -225,6 +246,14 @@
   </si>
   <si>
     <t xml:space="preserve">울트라 냥냥가챠 뽑기권 확률 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Item_Grade</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Acquired_Mileage</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -323,7 +352,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -684,6 +713,16 @@
 </ThreadedComments>
 </file>
 
+<file path=xl/threadedComments/threadedComment3.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A1" dT="2024-09-25T11:40:49.07" personId="{DEFDF8BA-08CC-4ECF-8F60-F1EEA043FDC6}" id="{262C3525-30B3-4A0E-9280-CCBF27DD5D25}">
+    <text>Normal = 1
+Rare = 2
+Unique = 3</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0A44DD5-7D06-438B-9FE5-436D9EFF504F}">
   <dimension ref="A1:I3"/>
@@ -692,16 +731,16 @@
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="16.3984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="15.69921875" customWidth="1"/>
+    <col min="4" max="7" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="15.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -730,7 +769,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>100011</v>
       </c>
@@ -759,7 +798,7 @@
         <v>73050</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>100012</v>
       </c>
@@ -800,18 +839,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BA63B6B-56B9-4D2F-ADF1-A0D874D69E23}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.09765625" customWidth="1"/>
-    <col min="2" max="2" width="26.796875" customWidth="1"/>
+    <col min="1" max="1" width="10.125" customWidth="1"/>
+    <col min="2" max="2" width="26.75" customWidth="1"/>
     <col min="3" max="6" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -831,7 +870,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1001001</v>
       </c>
@@ -851,7 +890,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1001002</v>
       </c>
@@ -871,7 +910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1001003</v>
       </c>
@@ -891,7 +930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1001004</v>
       </c>
@@ -911,7 +950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1001005</v>
       </c>
@@ -931,7 +970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1001006</v>
       </c>
@@ -951,7 +990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1001007</v>
       </c>
@@ -971,7 +1010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1001008</v>
       </c>
@@ -991,7 +1030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1001009</v>
       </c>
@@ -1011,7 +1050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1001010</v>
       </c>
@@ -1031,7 +1070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1001011</v>
       </c>
@@ -1051,7 +1090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1001012</v>
       </c>
@@ -1071,7 +1110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1001013</v>
       </c>
@@ -1091,7 +1130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1001014</v>
       </c>
@@ -1111,7 +1150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1001015</v>
       </c>
@@ -1131,7 +1170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1001016</v>
       </c>
@@ -1151,7 +1190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>1002001</v>
       </c>
@@ -1171,7 +1210,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>1002002</v>
       </c>
@@ -1191,7 +1230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>1002003</v>
       </c>
@@ -1211,7 +1250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>1002004</v>
       </c>
@@ -1231,7 +1270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>1002005</v>
       </c>
@@ -1251,7 +1290,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>1002006</v>
       </c>
@@ -1271,7 +1310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
         <v>1002007</v>
       </c>
@@ -1291,7 +1330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
         <v>1002008</v>
       </c>
@@ -1311,7 +1350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <v>1002009</v>
       </c>
@@ -1331,7 +1370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
         <v>1002010</v>
       </c>
@@ -1351,7 +1390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
         <v>1002011</v>
       </c>
@@ -1379,22 +1418,60 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC866BF9-E829-4339-BA0A-DDA95ECAF929}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="문서" ma:contentTypeID="0x0101000168296C255B5D46B72DA629862DD870" ma:contentTypeVersion="6" ma:contentTypeDescription="새 문서를 만듭니다." ma:contentTypeScope="" ma:versionID="a688b941d50903c1d18649d8c0763796">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="216f0c87-b1ea-4333-b2c4-608be75d64b1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ff4785467fc8158ecbe8e36ba569b54a" ns3:_="">
     <xsd:import namespace="216f0c87-b1ea-4333-b2c4-608be75d64b1"/>
@@ -1552,31 +1629,22 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3937CF16-5D2A-4290-A80F-934D1B2B013A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95EE4443-A78B-461C-B08E-5464C845DB42}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="216f0c87-b1ea-4333-b2c4-608be75d64b1"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62ACDFD5-C600-4A9D-A2FF-B29B86319DE6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1592,4 +1660,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95EE4443-A78B-461C-B08E-5464C845DB42}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="216f0c87-b1ea-4333-b2c4-608be75d64b1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3937CF16-5D2A-4290-A80F-934D1B2B013A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>